<commit_message>
chore(): add some specs
</commit_message>
<xml_diff>
--- a/resources/01-Banteay-Meanchey.xlsx
+++ b/resources/01-Banteay-Meanchey.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="204"/>
+    <workbookView xWindow="9880" yWindow="760" windowWidth="16660" windowHeight="11980" tabRatio="204" firstSheet="67" activeTab="75"/>
   </bookViews>
   <sheets>
     <sheet name="Page 1" sheetId="1" r:id="rId1"/>
@@ -2342,7 +2342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2841,15 +2841,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F9:J9"/>
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3595,15 +3595,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3618,7 +3618,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4406,22 +4408,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="C4:N4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -5216,15 +5218,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -6550,15 +6552,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -7445,15 +7447,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -8105,15 +8107,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -8767,15 +8769,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -9536,6 +9538,16 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="D4:N4"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A12:B12"/>
@@ -9543,16 +9555,6 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="D4:N4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -10440,15 +10442,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -11835,16 +11837,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="O10:P10"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -12702,15 +12704,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -13317,15 +13319,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -13984,22 +13986,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="D4:N4"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="D4:N4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -14568,21 +14570,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="C4:N4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -15234,15 +15236,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -16331,15 +16333,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -17290,15 +17292,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -17901,15 +17903,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -18562,16 +18564,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="O10:P10"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -19705,15 +19707,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -20176,16 +20178,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="O10:P10"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -20837,15 +20839,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -21892,16 +21894,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="F9:J9"/>
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="O11:P11"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -22598,15 +22600,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -23070,15 +23072,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -23685,15 +23687,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -24392,15 +24394,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -25816,15 +25818,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -26290,16 +26292,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="C4:N4"/>
     <mergeCell ref="E5:K5"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="G8:K8"/>
     <mergeCell ref="P8:R8"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="C4:N4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -26949,15 +26951,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -27750,15 +27752,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -33869,15 +33871,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -35113,17 +35115,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="P9:R9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="P3:R3"/>
     <mergeCell ref="D4:N4"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="P9:R9"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -35822,15 +35824,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -37154,15 +37156,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -37765,15 +37767,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -38425,15 +38427,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -38448,7 +38450,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -38946,16 +38950,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="O10:P10"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -40002,15 +40006,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -40615,15 +40619,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -42053,15 +42057,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -42671,15 +42675,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F9:J9"/>
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -43970,15 +43974,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -44584,15 +44588,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -45823,15 +45827,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -46683,15 +46687,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -47543,15 +47547,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -47566,7 +47570,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -48081,6 +48087,9 @@
       <c r="K18" s="2">
         <v>135</v>
       </c>
+      <c r="L18" s="2">
+        <v>0</v>
+      </c>
       <c r="M18" s="2">
         <v>13</v>
       </c>
@@ -48198,15 +48207,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -49113,15 +49122,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="F9:J9"/>
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -49882,15 +49891,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -50354,15 +50363,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -51155,15 +51164,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -52015,15 +52024,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -52441,15 +52450,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -53054,15 +53063,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -54007,15 +54016,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -54477,15 +54486,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -54956,16 +54965,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="C4:N4"/>
     <mergeCell ref="E5:K5"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="G9:K9"/>
     <mergeCell ref="P9:R9"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="C4:N4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -55962,15 +55971,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -56541,15 +56550,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -57011,15 +57020,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="C4:M4"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -57624,15 +57633,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -58344,15 +58353,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="B4:M4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F8:J8"/>
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -58739,14 +58748,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="C4:L4"/>
     <mergeCell ref="E5:I5"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="O2:P2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="C4:L4"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>